<commit_message>
ocultando campos direccion motivo en agregar documento y plantilla excel de carga de documentos
</commit_message>
<xml_diff>
--- a/public/templates/PlantillaCargaDocumentos.xlsx
+++ b/public/templates/PlantillaCargaDocumentos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\strat1\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\strat1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC7DAD2-00B2-4F9E-AAAC-E0CF8291FC84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418ADAFB-1C49-4526-8750-10DCB47E8DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="630" yWindow="3285" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cabecera" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="96">
   <si>
     <t>Fecha de Contabilización</t>
   </si>
@@ -320,9 +320,6 @@
   </si>
   <si>
     <t>TIPO IMPUESTO</t>
-  </si>
-  <si>
-    <t>Direccion</t>
   </si>
   <si>
     <t>Indicador de Impuesto</t>
@@ -545,7 +542,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -615,9 +612,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -933,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -953,12 +947,11 @@
     <col min="10" max="10" width="24.140625" style="7" customWidth="1"/>
     <col min="11" max="11" width="24.42578125" style="7" customWidth="1"/>
     <col min="12" max="12" width="20.140625" style="7" customWidth="1"/>
-    <col min="13" max="13" width="23.42578125" style="7" customWidth="1"/>
-    <col min="14" max="14" width="16" style="7" customWidth="1"/>
-    <col min="16" max="16" width="11.42578125" customWidth="1"/>
+    <col min="13" max="13" width="16" style="7" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="49.5" customHeight="1">
+    <row r="1" spans="1:14" ht="49.5" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>62</v>
       </c>
@@ -995,14 +988,11 @@
       <c r="L1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="N1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="13" customFormat="1">
+    <row r="2" spans="1:14" s="13" customFormat="1">
       <c r="A2" s="14"/>
       <c r="B2" s="28"/>
       <c r="C2" s="16"/>
@@ -1016,9 +1006,8 @@
       <c r="K2" s="32"/>
       <c r="L2" s="14"/>
       <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-    </row>
-    <row r="3" spans="1:15" s="15" customFormat="1">
+    </row>
+    <row r="3" spans="1:14" s="15" customFormat="1">
       <c r="A3" s="14"/>
       <c r="B3" s="28"/>
       <c r="C3" s="16"/>
@@ -1032,12 +1021,10 @@
       <c r="K3" s="32"/>
       <c r="L3" s="14"/>
       <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-    </row>
-    <row r="4" spans="1:15" s="15" customFormat="1">
+    </row>
+    <row r="4" spans="1:14" s="15" customFormat="1">
       <c r="A4" s="14"/>
       <c r="B4" s="28"/>
-      <c r="C4" s="16"/>
       <c r="D4" s="16"/>
       <c r="E4" s="17"/>
       <c r="F4" s="14"/>
@@ -1048,9 +1035,8 @@
       <c r="K4" s="32"/>
       <c r="L4" s="14"/>
       <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-    </row>
-    <row r="5" spans="1:15">
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="14"/>
       <c r="B5" s="28"/>
       <c r="C5" s="16"/>
@@ -1064,9 +1050,8 @@
       <c r="K5" s="32"/>
       <c r="L5" s="14"/>
       <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-    </row>
-    <row r="6" spans="1:15" s="19" customFormat="1">
+    </row>
+    <row r="6" spans="1:14" s="19" customFormat="1">
       <c r="A6" s="31"/>
       <c r="B6" s="30"/>
       <c r="C6" s="21"/>
@@ -1080,23 +1065,22 @@
       <c r="K6" s="20"/>
       <c r="L6" s="20"/>
       <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-    </row>
-    <row r="7" spans="1:15">
+    </row>
+    <row r="7" spans="1:14">
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
-      <c r="O7" s="8"/>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="N7" s="8"/>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="10"/>
-      <c r="C8" s="11"/>
+      <c r="C8" s="16"/>
       <c r="D8" s="11"/>
       <c r="E8" s="12"/>
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M5 H2:H5" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H5" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>254</formula1>
     </dataValidation>
     <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J5" xr:uid="{00000000-0002-0000-0000-000001000000}">
@@ -1108,7 +1092,7 @@
     <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L5" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>1E+22</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:E1048576" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:E3 D4:E4 C5:E1048576" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>36161</formula1>
     </dataValidation>
   </dataValidations>
@@ -1121,7 +1105,7 @@
           <x14:formula1>
             <xm:f>'TIPOS-LISTAS'!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>N2:N1048576</xm:sqref>
+          <xm:sqref>M2:M1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6C754A37-D63F-477F-AD2F-ACE794A0519B}">
           <x14:formula1>
@@ -1171,10 +1155,10 @@
         <v>54</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>95</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>55</v>
@@ -1295,32 +1279,26 @@
       <c r="B1" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="44"/>
       <c r="D1" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="44"/>
       <c r="F1" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="45"/>
       <c r="H1" s="42" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="2:8">
       <c r="B2" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="44"/>
       <c r="D2" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="44"/>
       <c r="F2" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="G2" s="45"/>
       <c r="H2" s="38" t="s">
         <v>10</v>
       </c>
@@ -1329,15 +1307,12 @@
       <c r="B3" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="44"/>
       <c r="D3" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="44"/>
       <c r="F3" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="45"/>
       <c r="H3" s="38" t="s">
         <v>11</v>
       </c>
@@ -1346,181 +1321,87 @@
       <c r="B4" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="44"/>
       <c r="D4" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="E4" s="44"/>
       <c r="F4" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="G4" s="45"/>
-      <c r="H4" s="43"/>
     </row>
     <row r="5" spans="2:8">
-      <c r="B5" s="43"/>
-      <c r="C5" s="44"/>
       <c r="D5" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="44"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="43"/>
     </row>
     <row r="6" spans="2:8">
-      <c r="B6" s="43"/>
-      <c r="C6" s="44"/>
       <c r="D6" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="E6" s="44"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="43"/>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="43"/>
-      <c r="C7" s="44"/>
       <c r="D7" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="E7" s="44"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="43"/>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="43"/>
-      <c r="C8" s="44"/>
       <c r="D8" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="E8" s="44"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="43"/>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" s="43"/>
-      <c r="C9" s="44"/>
       <c r="D9" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="E9" s="44"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="43"/>
     </row>
     <row r="10" spans="2:8">
-      <c r="B10" s="43"/>
-      <c r="C10" s="44"/>
       <c r="D10" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="E10" s="44"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="43"/>
     </row>
     <row r="11" spans="2:8">
-      <c r="B11" s="43"/>
-      <c r="C11" s="44"/>
       <c r="D11" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="E11" s="44"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="43"/>
     </row>
     <row r="12" spans="2:8">
-      <c r="B12" s="43"/>
-      <c r="C12" s="44"/>
       <c r="D12" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="E12" s="44"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="43"/>
     </row>
     <row r="13" spans="2:8">
-      <c r="B13" s="43"/>
-      <c r="C13" s="44"/>
       <c r="D13" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="E13" s="44"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="43"/>
     </row>
     <row r="14" spans="2:8">
-      <c r="B14" s="43"/>
-      <c r="C14" s="44"/>
       <c r="D14" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="E14" s="44"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="43"/>
     </row>
     <row r="15" spans="2:8">
-      <c r="B15" s="43"/>
-      <c r="C15" s="44"/>
       <c r="D15" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="E15" s="44"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="43"/>
     </row>
     <row r="16" spans="2:8">
-      <c r="B16" s="43"/>
-      <c r="C16" s="44"/>
       <c r="D16" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="E16" s="44"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="43"/>
-    </row>
-    <row r="17" spans="2:8">
-      <c r="B17" s="43"/>
-      <c r="C17" s="44"/>
+    </row>
+    <row r="17" spans="4:4">
       <c r="D17" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="44"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="43"/>
-    </row>
-    <row r="18" spans="2:8">
-      <c r="B18" s="43"/>
-      <c r="C18" s="44"/>
+    </row>
+    <row r="18" spans="4:4">
       <c r="D18" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="44"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="43"/>
-    </row>
-    <row r="19" spans="2:8">
-      <c r="B19" s="43"/>
-      <c r="C19" s="44"/>
+    </row>
+    <row r="19" spans="4:4">
       <c r="D19" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="E19" s="44"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="43"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feature | plantilla de importacion actualizada - fix | bugs al mostrar los footer de Monto Total correspondientes
</commit_message>
<xml_diff>
--- a/public/templates/PlantillaCargaDocumentos.xlsx
+++ b/public/templates/PlantillaCargaDocumentos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\strat1\Desktop\EXCELS IMPORTACION DOCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C25F984-5AFD-4A6E-BAB0-5ACC87044C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2A8F83-F276-4B74-97B7-D16E4E9439B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="2490" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cabecera" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <definedName name="TIPOAFECTACION">'TIPOS-LISTAS'!$B$2:$B$4</definedName>
     <definedName name="TipoDocs">#REF!</definedName>
     <definedName name="TIPODOCUMENTO">'TIPOS-LISTAS'!$D$2:$D$18</definedName>
-    <definedName name="TIPOIMPUESTO">'TIPOS-LISTAS'!$F$2:$F$4</definedName>
+    <definedName name="TIPOIMPUESTO">'TIPOS-LISTAS'!$F$2:$F$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -207,10 +207,10 @@
     <t>Importe Total</t>
   </si>
   <si>
-    <t>EXO - No domiciliados (24%)</t>
-  </si>
-  <si>
-    <t>EXO - Recibo por honorarios (8%)</t>
+    <t>IGV_GAST - IGV GASTO</t>
+  </si>
+  <si>
+    <t>IGV_MIXT - IGV MIXTO</t>
   </si>
 </sst>
 </file>
@@ -783,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,7 +1144,7 @@
   <dimension ref="B1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1205,7 +1205,7 @@
         <v>32</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1221,7 +1221,7 @@
         <v>34</v>
       </c>
       <c r="F6" s="32" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feature | modificaciones realizadaa al archivo excel de la importacion de plantilla
</commit_message>
<xml_diff>
--- a/public/templates/PlantillaCargaDocumentos.xlsx
+++ b/public/templates/PlantillaCargaDocumentos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\strat1\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\strat1\Documents\ear\ear-crl\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E19D471-987A-4BF3-90A8-C9EA22F097E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9AA02C-3077-4E8F-8C96-8D72B33E17B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,8 +27,8 @@
     <definedName name="Opciones1">#REF!</definedName>
     <definedName name="TIPOAFECTACION">'TIPOS-LISTAS'!$B$2:$B$4</definedName>
     <definedName name="TipoDocs">#REF!</definedName>
-    <definedName name="TIPODOCUMENTO">'TIPOS-LISTAS'!$D$2:$D$18</definedName>
-    <definedName name="TIPOIMPUESTO">'TIPOS-LISTAS'!$F$2:$F$6</definedName>
+    <definedName name="TIPODOCUMENTO">'TIPOS-LISTAS'!$D$2:$D$20</definedName>
+    <definedName name="TIPOIMPUESTO">'TIPOS-LISTAS'!$F$2:$F$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -108,24 +108,12 @@
     <t>N° Documento</t>
   </si>
   <si>
-    <t>1 - Retencion</t>
-  </si>
-  <si>
-    <t>2 - Detraccion</t>
-  </si>
-  <si>
     <t>Afectacion</t>
   </si>
   <si>
-    <t>IGV_LEY - IGV (10%)</t>
-  </si>
-  <si>
     <t>IGV - IGV (18%)</t>
   </si>
   <si>
-    <t>EXO - EXO</t>
-  </si>
-  <si>
     <t>SUBTOTAL</t>
   </si>
   <si>
@@ -147,9 +135,6 @@
     <t>06 - Carga porte aereo</t>
   </si>
   <si>
-    <t>10 - Recibo por arrendamiento</t>
-  </si>
-  <si>
     <t>11 - Poliza de bolsa de valores</t>
   </si>
   <si>
@@ -204,19 +189,34 @@
     <t>Importe Total</t>
   </si>
   <si>
-    <t>IGV_GAST - IGV GASTO</t>
-  </si>
-  <si>
-    <t>IGV_MIXT - IGV MIXTO</t>
-  </si>
-  <si>
-    <t>5 - -</t>
-  </si>
-  <si>
     <t>4 - Recibo por honorarios</t>
   </si>
   <si>
     <t>3 - No domiciliados</t>
+  </si>
+  <si>
+    <t>1 - Retención</t>
+  </si>
+  <si>
+    <t>2 - Detracción</t>
+  </si>
+  <si>
+    <t>5 - Ninguno</t>
+  </si>
+  <si>
+    <t>07 - Nota de credito</t>
+  </si>
+  <si>
+    <t>08 - Nota de debito</t>
+  </si>
+  <si>
+    <t>10 - Recibo de arrendamiento</t>
+  </si>
+  <si>
+    <t>IGV_LEY - IGV LEY</t>
+  </si>
+  <si>
+    <t>EXO - Exonerado</t>
   </si>
 </sst>
 </file>
@@ -397,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -423,14 +423,13 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify"/>
     </xf>
@@ -751,7 +750,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,7 +768,7 @@
         <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -799,18 +798,18 @@
         <v>7</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19"/>
       <c r="B2" s="19"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
@@ -823,9 +822,9 @@
     <row r="3" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
       <c r="B3" s="19"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
       <c r="H3" s="19"/>
@@ -838,9 +837,9 @@
     <row r="4" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
       <c r="B4" s="19"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
       <c r="F4" s="19"/>
       <c r="G4" s="19"/>
       <c r="H4" s="19"/>
@@ -851,17 +850,17 @@
       <c r="M4" s="19"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
       <c r="K5" s="22"/>
     </row>
     <row r="6" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="19"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
       <c r="H6" s="19"/>
@@ -869,37 +868,37 @@
       <c r="J6" s="20"/>
       <c r="K6" s="22"/>
       <c r="L6" s="19"/>
-      <c r="M6" s="25"/>
+      <c r="M6" s="24"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
       <c r="K7" s="22"/>
       <c r="N7" s="3"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
       <c r="K8" s="22"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
       <c r="K9" s="22"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
       <c r="K10" s="22"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
       <c r="K11" s="22"/>
     </row>
   </sheetData>
@@ -940,7 +939,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{96122AA3-8AEE-428C-9A32-41319D4B5DD6}">
           <x14:formula1>
-            <xm:f>'TIPOS-LISTAS'!$D$2:$D$18</xm:f>
+            <xm:f>'TIPOS-LISTAS'!$D$2:$D$20</xm:f>
           </x14:formula1>
           <xm:sqref>I2:I1048576</xm:sqref>
         </x14:dataValidation>
@@ -955,7 +954,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:M1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,10 +981,10 @@
         <v>13</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>14</v>
@@ -1009,7 +1008,7 @@
         <v>17</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1149,7 +1148,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9D437790-D5E3-41BC-B587-1D0FBB095C4E}">
           <x14:formula1>
-            <xm:f>'TIPOS-LISTAS'!$F$2:$F$6</xm:f>
+            <xm:f>'TIPOS-LISTAS'!$F$2:$F$4</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
@@ -1161,10 +1160,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82BE67A2-D4B7-4910-9C63-2E887AFCDE76}">
-  <dimension ref="B1:H18"/>
+  <dimension ref="B1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,27 +1176,27 @@
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="16" t="s">
         <v>46</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>9</v>
@@ -1205,13 +1204,13 @@
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>10</v>
@@ -1219,95 +1218,99 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>58</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D7" s="10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D8" s="10" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D9" s="10" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D10" s="10" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D11" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D12" s="10" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D13" s="10" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D14" s="10" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D15" s="10" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D16" s="10" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="10" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="10" t="s">
-        <v>45</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="10" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: mejora en la exportacion de detalles form documento
</commit_message>
<xml_diff>
--- a/public/templates/PlantillaCargaDocumentos.xlsx
+++ b/public/templates/PlantillaCargaDocumentos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\strat1\Documents\ear\ear-crl\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9AA02C-3077-4E8F-8C96-8D72B33E17B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B4C4CB-9A72-49EF-86D3-F82E1399461E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22995" yWindow="3150" windowWidth="20385" windowHeight="11550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cabecera" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <definedName name="Opciones1">#REF!</definedName>
     <definedName name="TIPOAFECTACION">'TIPOS-LISTAS'!$B$2:$B$4</definedName>
     <definedName name="TipoDocs">#REF!</definedName>
-    <definedName name="TIPODOCUMENTO">'TIPOS-LISTAS'!$D$2:$D$20</definedName>
+    <definedName name="TIPODOCUMENTO">'TIPOS-LISTAS'!$D$2:$D$18</definedName>
     <definedName name="TIPOIMPUESTO">'TIPOS-LISTAS'!$F$2:$F$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Fecha de Contabilización</t>
   </si>
@@ -202,12 +202,6 @@
   </si>
   <si>
     <t>5 - Ninguno</t>
-  </si>
-  <si>
-    <t>07 - Nota de credito</t>
-  </si>
-  <si>
-    <t>08 - Nota de debito</t>
   </si>
   <si>
     <t>10 - Recibo de arrendamiento</t>
@@ -939,7 +933,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{96122AA3-8AEE-428C-9A32-41319D4B5DD6}">
           <x14:formula1>
-            <xm:f>'TIPOS-LISTAS'!$D$2:$D$20</xm:f>
+            <xm:f>'TIPOS-LISTAS'!$D$2:$D$18</xm:f>
           </x14:formula1>
           <xm:sqref>I2:I1048576</xm:sqref>
         </x14:dataValidation>
@@ -1160,16 +1154,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82BE67A2-D4B7-4910-9C63-2E887AFCDE76}">
-  <dimension ref="B1:H20"/>
+  <dimension ref="B1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1210,7 +1204,7 @@
         <v>26</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>10</v>
@@ -1224,7 +1218,7 @@
         <v>27</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1255,61 +1249,51 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D9" s="10" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D10" s="10" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D11" s="10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D12" s="10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D13" s="10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D14" s="10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D15" s="10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D16" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D19" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D20" s="10" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>